<commit_message>
feat(example): improve nightfall enemy lookup and add vite dev server
</commit_message>
<xml_diff>
--- a/example/game_06_abyssal_nightfall/waves.xlsx
+++ b/example/game_06_abyssal_nightfall/waves.xlsx
@@ -419,7 +419,7 @@
         <v>uint</v>
       </c>
       <c r="F4" t="str">
-        <v>string</v>
+        <v>tid</v>
       </c>
       <c r="G4" t="str">
         <v>uint</v>
@@ -483,7 +483,7 @@
         <v>30</v>
       </c>
       <c r="F6" t="str">
-        <v>enemy:shambler</v>
+        <v>40060001</v>
       </c>
       <c r="G6" t="str">
         <v>18</v>
@@ -515,7 +515,7 @@
         <v>40</v>
       </c>
       <c r="F7" t="str">
-        <v>enemy:cultist</v>
+        <v>40060002</v>
       </c>
       <c r="G7" t="str">
         <v>12</v>
@@ -547,7 +547,7 @@
         <v>35</v>
       </c>
       <c r="F8" t="str">
-        <v>enemy:abyssal-howler</v>
+        <v>40060003</v>
       </c>
       <c r="G8" t="str">
         <v>8</v>
@@ -579,7 +579,7 @@
         <v>45</v>
       </c>
       <c r="F9" t="str">
-        <v>enemy:null-sentinel</v>
+        <v>40060004</v>
       </c>
       <c r="G9" t="str">
         <v>5</v>
@@ -611,7 +611,7 @@
         <v>40</v>
       </c>
       <c r="F10" t="str">
-        <v>enemy:myriad-fragment</v>
+        <v>40060006</v>
       </c>
       <c r="G10" t="str">
         <v>16</v>
@@ -643,7 +643,7 @@
         <v>50</v>
       </c>
       <c r="F11" t="str">
-        <v>enemy:harbor-dredger</v>
+        <v>40060005</v>
       </c>
       <c r="G11" t="str">
         <v>6</v>

</xml_diff>